<commit_message>
~Updated "Add person" forms ~~utilizes builtin form functionalities ~~ride choosing uses select instead of radio inputs ~~gives invalid input warning if submitted improperly ~~resets form after successful submission ~changed dev port from 3000 to 4000 ~updated placeholder sheet ~Restyled footer to be left aligned ~Restyled most pages to end with footer on bottom without need for scrolling
</commit_message>
<xml_diff>
--- a/public/placeholdersheet.xlsx
+++ b/public/placeholdersheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0893e936dbe216fc/Documents/CodeProjects/RidesProjectVA/ride-organizer-va/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_5413CE126337C6C81B22ABD9951E03F5312588FA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4CE0B517-301C-47CC-BDC8-403F3C4D0E29}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="11_6431EACCB51D5CEC531FE149149C838CD3A222C4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E4871757-8BFB-47C1-B307-68D5637CCCC1}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Passenger Form Responses" sheetId="1" r:id="rId1"/>
@@ -20,70 +20,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Georgia"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>Responder updated this value.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Georgia"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>Responder updated this value.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Georgia"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>Responder updated this value.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Georgia"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>Responder updated this value.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="72">
   <si>
     <t>Timestamp</t>
   </si>
@@ -115,106 +53,196 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>agee4@uci.edu</t>
-  </si>
-  <si>
-    <t>Bob Billigan</t>
-  </si>
-  <si>
-    <t>555 555 5555</t>
-  </si>
-  <si>
     <t>Sunday Third Service 11:30am</t>
   </si>
   <si>
-    <t>112 Stanford Ct</t>
-  </si>
-  <si>
     <t>UCI</t>
   </si>
   <si>
+    <t>Freshman</t>
+  </si>
+  <si>
     <t>Sophomore</t>
   </si>
   <si>
-    <t>I do not exist ):</t>
-  </si>
-  <si>
-    <t>Tombert Johndoe</t>
-  </si>
-  <si>
-    <t>123 456 7890</t>
-  </si>
-  <si>
     <t>Friday Bible Study 7:00pm, Sunday First Service 8:00am</t>
   </si>
   <si>
-    <t>287 Berkeley Ave</t>
-  </si>
-  <si>
     <t>Junior</t>
   </si>
   <si>
-    <t>Sunday Second Service 9:30am, Sunday Third Service 11:30am</t>
-  </si>
-  <si>
     <t>Planning on taking membership class</t>
   </si>
   <si>
-    <t>Gaius Algersyn</t>
-  </si>
-  <si>
-    <t>955 758 3619</t>
+    <t>pass1@ryd.org</t>
+  </si>
+  <si>
+    <t>Passenger 1</t>
+  </si>
+  <si>
+    <t>111 555 1234</t>
+  </si>
+  <si>
+    <t>Sunday First Service 8:00am</t>
+  </si>
+  <si>
+    <t>455 Cornell</t>
+  </si>
+  <si>
+    <t>pass2@ryd.org</t>
+  </si>
+  <si>
+    <t>Passenger 2</t>
+  </si>
+  <si>
+    <t>112 555 1234</t>
   </si>
   <si>
     <t>Friday Bible Study 7:00pm, Sunday Second Service 9:30am</t>
   </si>
   <si>
-    <t>53 Dartmouth</t>
-  </si>
-  <si>
-    <t>Senior</t>
-  </si>
-  <si>
-    <t>Aaron Gee</t>
-  </si>
-  <si>
-    <t>916 385 7559</t>
-  </si>
-  <si>
-    <t>292 Tustin Field Dr</t>
-  </si>
-  <si>
-    <t>Out of School</t>
+    <t>267 Berkeley Ave</t>
+  </si>
+  <si>
+    <t>pass3@ryd.org</t>
+  </si>
+  <si>
+    <t>Passenger 3</t>
+  </si>
+  <si>
+    <t>113 555 1234</t>
+  </si>
+  <si>
+    <t>Sunday Second Service 9:30am</t>
+  </si>
+  <si>
+    <t>1642 Stanford Ct</t>
+  </si>
+  <si>
+    <t>pass4@ryd.org</t>
+  </si>
+  <si>
+    <t>Passenger 4</t>
+  </si>
+  <si>
+    <t>114 555 1234</t>
+  </si>
+  <si>
+    <t>207 Cornell</t>
+  </si>
+  <si>
+    <t>pass5@ryd.org</t>
+  </si>
+  <si>
+    <t>Passenger 5</t>
+  </si>
+  <si>
+    <t>115 555 1234</t>
+  </si>
+  <si>
+    <t>Friday Bible Study 7:00pm, Sunday Third Service 11:30am</t>
+  </si>
+  <si>
+    <t>Middle Earth</t>
+  </si>
+  <si>
+    <t>pass6@ryd.org</t>
+  </si>
+  <si>
+    <t>Passenger 6</t>
+  </si>
+  <si>
+    <t>116 555 1234</t>
+  </si>
+  <si>
+    <t>Mesa</t>
+  </si>
+  <si>
+    <t>pass7@ryd.org</t>
+  </si>
+  <si>
+    <t>Passenger 7</t>
+  </si>
+  <si>
+    <t>117 555 1234</t>
+  </si>
+  <si>
+    <t>6501 E De Leon St</t>
+  </si>
+  <si>
+    <t>CSULB</t>
   </si>
   <si>
     <t>Seats</t>
   </si>
   <si>
-    <t>Trebor Tenfingers</t>
-  </si>
-  <si>
-    <t>9358 Lufkin Way</t>
-  </si>
-  <si>
-    <t>I got a pet goose.</t>
-  </si>
-  <si>
-    <t>070 925 2002</t>
+    <t>driv1@ryd.org</t>
+  </si>
+  <si>
+    <t>Driver 1</t>
+  </si>
+  <si>
+    <t>111 555 4321</t>
+  </si>
+  <si>
+    <t>283 Berkeley Ave</t>
+  </si>
+  <si>
+    <t>Driver 2</t>
+  </si>
+  <si>
+    <t>112 555 4321</t>
+  </si>
+  <si>
+    <t>6502 E De Leon St</t>
+  </si>
+  <si>
+    <t>135 Cornell</t>
+  </si>
+  <si>
+    <t>driv2@ryd.org</t>
+  </si>
+  <si>
+    <t>1454 Stanford Ct</t>
+  </si>
+  <si>
+    <t>Can't drive back</t>
+  </si>
+  <si>
+    <t>driv3@ryd.org</t>
+  </si>
+  <si>
+    <t>Driver 3</t>
+  </si>
+  <si>
+    <t>113 555 4321</t>
+  </si>
+  <si>
+    <t>driv4@ryd.org</t>
+  </si>
+  <si>
+    <t>Driver 4</t>
+  </si>
+  <si>
+    <t>114 555 4321</t>
+  </si>
+  <si>
+    <t>Passenger 8</t>
+  </si>
+  <si>
+    <t>118 555 1234</t>
   </si>
   <si>
     <t>Friday Bible Study 7:00pm</t>
   </si>
   <si>
-    <t>no.</t>
+    <t>22000 Arroyo Dr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -237,7 +265,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -412,54 +440,87 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF442F65"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFFFFFFF"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF442F65"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFFFFFFF"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFFFFFFF"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF442F65"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFFFFFFF"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF442F65"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF442F65"/>
-      </bottom>
+        <color rgb="FFF8F9FA"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF442F65"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFF8F9FA"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF442F65"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF442F65"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF442F65"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF442F65"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF442F65"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF442F65"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF442F65"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF442F65"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -470,37 +531,49 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -580,8 +653,12 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:J5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Passengers" displayName="Passengers" ref="A1:J9">
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Timestamp"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Email Address"/>
@@ -599,7 +676,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Form_Responses2" displayName="Form_Responses2" ref="A1:I2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Drivers" displayName="Drivers" ref="A1:I5">
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Timestamp"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Email Address"/>
@@ -812,15 +889,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -869,130 +946,238 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
-        <v>45722.759284756947</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="5" t="s">
+      <c r="A2" s="8">
+        <v>45728</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="5" t="s">
+      <c r="H2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="6"/>
+      <c r="J2" s="7" t="s">
         <v>16</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7">
-        <v>45722.759111296298</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="8" t="s">
+      <c r="A3" s="9">
+        <v>45729</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="9" t="s">
-        <v>24</v>
-      </c>
+      <c r="I3" s="4"/>
+      <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
-        <v>45722.760744780091</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="A4" s="8">
+        <v>45730</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>29</v>
+      <c r="J4" s="7" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="10">
-        <v>45727.747038946763</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="11" t="s">
+      <c r="A5" s="9">
+        <v>45731</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="G5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="5"/>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="8">
+        <v>45732</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E6" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F5" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="I5" s="11"/>
-      <c r="J5" s="14" t="s">
-        <v>37</v>
-      </c>
+      <c r="F6" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="7"/>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="9">
+        <v>45733</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" s="5"/>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="16">
+        <v>45734</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="17"/>
+      <c r="J8" s="18"/>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="10">
+        <v>45735</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1002,11 +1187,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1028,7 +1213,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>6</v>
@@ -1044,38 +1229,120 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12">
-        <v>45727.940887303237</v>
-      </c>
-      <c r="B2" s="13" t="s">
+      <c r="A2" s="8">
+        <v>45728</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="6">
+        <v>4</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="7"/>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="16">
+        <v>45729</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="17">
+        <v>4</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="I3" s="18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="16">
+        <v>45730</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" s="17">
+        <v>4</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="13">
+      <c r="H4" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="I4" s="18"/>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="13">
+        <v>45731</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="14">
         <v>4</v>
       </c>
-      <c r="F2" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="I2" t="s">
-        <v>40</v>
-      </c>
+      <c r="F5" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="I5" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Proper Ride Loading & Dynamic Processing stuff
+loadsheet can now properly build rides
~updated placeholdersheet (again) to be more "realistic"
+createpassengerform can set year
~updated createpeopleforms to dynamically generate option forms based on enums
~ridemanager filter display slightly changed
+begun implementation of dragging passengers already in a ride (^todo: add dragging ride passengers either to unassigned list, fix dragging to another ride not removing from previous ride)
~refactored loadsheet to be more flexible in parsing data to build people
+added field to customize savesheet name
</commit_message>
<xml_diff>
--- a/public/placeholdersheet.xlsx
+++ b/public/placeholdersheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="138">
   <si>
     <t>Timestamp</t>
   </si>
@@ -202,6 +202,9 @@
     <t>Senior</t>
   </si>
   <si>
+    <t>Thank you!! :DD</t>
+  </si>
+  <si>
     <t>pass10@ryd.org</t>
   </si>
   <si>
@@ -277,6 +280,9 @@
     <t>126 555 1234</t>
   </si>
   <si>
+    <t>Don't need a ride on the 17th</t>
+  </si>
+  <si>
     <t>pass17@ryd.org</t>
   </si>
   <si>
@@ -383,6 +389,9 @@
   </si>
   <si>
     <t>21000 Arroyo Dr</t>
+  </si>
+  <si>
+    <t>I have servant team meetings after third</t>
   </si>
   <si>
     <t>driv6@ryd.org</t>
@@ -722,7 +731,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="56">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -789,14 +798,17 @@
     <xf borderId="8" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="center"/>
     </xf>
+    <xf borderId="6" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="9" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
     <xf borderId="9" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf borderId="6" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="5" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="center"/>
@@ -845,34 +857,38 @@
     <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf borderId="5" fillId="3" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="5" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="16" fillId="0" fontId="1" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="17" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="17" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="18" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
     <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="5" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="16" fillId="0" fontId="1" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="17" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="17" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="18" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -917,11 +933,19 @@
       <border/>
     </dxf>
   </dxfs>
-  <tableStyles count="1">
+  <tableStyles count="3">
     <tableStyle count="3" pivot="0" name="Driver Form Responses-style">
       <tableStyleElement dxfId="1" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
       <tableStyleElement dxfId="3" type="secondRowStripe"/>
+    </tableStyle>
+    <tableStyle count="2" pivot="0" name="Driver Form Responses-style 2">
+      <tableStyleElement dxfId="3" type="firstRowStripe"/>
+      <tableStyleElement dxfId="2" type="secondRowStripe"/>
+    </tableStyle>
+    <tableStyle count="2" pivot="0" name="Driver Form Responses-style 3">
+      <tableStyleElement dxfId="3" type="firstRowStripe"/>
+      <tableStyleElement dxfId="2" type="secondRowStripe"/>
     </tableStyle>
   </tableStyles>
 </styleSheet>
@@ -949,6 +973,25 @@
     <tableColumn name="Notes" id="9"/>
   </tableColumns>
   <tableStyleInfo name="Driver Form Responses-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="B11:B15" displayName="Table_2" name="Table_2" id="2">
+  <tableColumns count="1">
+    <tableColumn name="Column1" id="1"/>
+  </tableColumns>
+  <tableStyleInfo name="Driver Form Responses-style 2" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="G11:H13" displayName="Table_3" name="Table_3" id="3">
+  <tableColumns count="2">
+    <tableColumn name="Column1" id="1"/>
+    <tableColumn name="Column2" id="2"/>
+  </tableColumns>
+  <tableStyleInfo name="Driver Form Responses-style 3" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
 </file>
 
@@ -1202,7 +1245,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" ht="15.75" hidden="1" customHeight="1">
+    <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="4">
         <v>45728.0</v>
       </c>
@@ -1322,7 +1365,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" ht="15.75" hidden="1" customHeight="1">
+    <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="4">
         <v>45732.0</v>
       </c>
@@ -1350,7 +1393,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="16"/>
     </row>
-    <row r="7" ht="15.75" hidden="1" customHeight="1">
+    <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="9">
         <v>45733.0</v>
       </c>
@@ -1406,9 +1449,11 @@
         <v>16</v>
       </c>
       <c r="I8" s="19"/>
-      <c r="J8" s="22"/>
+      <c r="J8" s="8" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="9" ht="15.75" hidden="1" customHeight="1">
+    <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="9">
         <v>45735.0</v>
       </c>
@@ -1434,11 +1479,9 @@
         <v>23</v>
       </c>
       <c r="I9" s="11"/>
-      <c r="J9" s="23" t="s">
-        <v>17</v>
-      </c>
+      <c r="J9" s="22"/>
     </row>
-    <row r="10" ht="15.75" hidden="1" customHeight="1">
+    <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="17">
         <v>45736.0</v>
       </c>
@@ -1466,26 +1509,28 @@
       <c r="I10" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="J10" s="22"/>
+      <c r="J10" s="23" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="11" ht="15.75" hidden="1" customHeight="1">
+    <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="9">
         <v>45737.0</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E11" s="12" t="s">
         <v>55</v>
       </c>
       <c r="F11" s="24" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G11" s="12" t="s">
         <v>51</v>
@@ -1496,18 +1541,18 @@
       <c r="I11" s="11"/>
       <c r="J11" s="13"/>
     </row>
-    <row r="12" ht="15.75" hidden="1" customHeight="1">
+    <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="17">
         <v>45738.0</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E12" s="21" t="s">
         <v>55</v>
@@ -1522,20 +1567,20 @@
         <v>40</v>
       </c>
       <c r="I12" s="19"/>
-      <c r="J12" s="22"/>
+      <c r="J12" s="25"/>
     </row>
-    <row r="13" ht="15.75" hidden="1" customHeight="1">
+    <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="9">
         <v>45739.0</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E13" s="14" t="s">
         <v>38</v>
@@ -1552,59 +1597,59 @@
       <c r="I13" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="J13" s="23" t="s">
+      <c r="J13" s="22" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" ht="15.75" hidden="1" customHeight="1">
+    <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="17">
         <v>45740.0</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E14" s="21" t="s">
         <v>55</v>
       </c>
       <c r="F14" s="21" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G14" s="21" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H14" s="21" t="s">
         <v>16</v>
       </c>
       <c r="I14" s="19"/>
-      <c r="J14" s="22"/>
+      <c r="J14" s="25"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="9">
         <v>45741.0</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E15" s="12" t="s">
         <v>27</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H15" s="12" t="s">
         <v>23</v>
@@ -1617,19 +1662,19 @@
         <v>45742.0</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E16" s="21" t="s">
         <v>27</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G16" s="21" t="s">
         <v>51</v>
@@ -1638,22 +1683,22 @@
         <v>40</v>
       </c>
       <c r="I16" s="19"/>
-      <c r="J16" s="22"/>
+      <c r="J16" s="25"/>
     </row>
-    <row r="17" ht="15.75" hidden="1" customHeight="1">
+    <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="9">
         <v>45743.0</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="E17" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="E17" s="26" t="s">
         <v>29</v>
       </c>
       <c r="F17" s="14" t="s">
@@ -1668,50 +1713,52 @@
       <c r="I17" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="J17" s="13"/>
+      <c r="J17" s="15" t="s">
+        <v>88</v>
+      </c>
     </row>
-    <row r="18" ht="15.75" hidden="1" customHeight="1">
+    <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="17">
         <v>45744.0</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E18" s="19" t="s">
         <v>44</v>
       </c>
       <c r="F18" s="21" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G18" s="21" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="H18" s="21" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="I18" s="19"/>
-      <c r="J18" s="22"/>
+      <c r="J18" s="25"/>
     </row>
-    <row r="19" ht="15.75" hidden="1" customHeight="1">
+    <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="9">
         <v>45745.0</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="E19" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="E19" s="26" t="s">
         <v>29</v>
       </c>
       <c r="F19" s="12" t="s">
@@ -1726,18 +1773,18 @@
       <c r="I19" s="11"/>
       <c r="J19" s="13"/>
     </row>
-    <row r="20" ht="15.75" hidden="1" customHeight="1">
+    <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="17">
         <v>45746.0</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E20" s="19" t="s">
         <v>44</v>
@@ -1752,49 +1799,49 @@
         <v>40</v>
       </c>
       <c r="I20" s="19"/>
-      <c r="J20" s="22"/>
+      <c r="J20" s="25"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="26">
+      <c r="A21" s="27">
         <v>45747.0</v>
       </c>
-      <c r="B21" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="C21" s="28" t="s">
-        <v>99</v>
-      </c>
-      <c r="D21" s="28" t="s">
+      <c r="B21" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="E21" s="28" t="s">
+      <c r="C21" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="D21" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="E21" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="F21" s="28" t="s">
+      <c r="F21" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="G21" s="29" t="s">
+      <c r="G21" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="H21" s="29" t="s">
+      <c r="H21" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="I21" s="28" t="s">
+      <c r="I21" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="J21" s="30"/>
+      <c r="J21" s="31"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="31"/>
+      <c r="A22" s="32"/>
       <c r="B22" s="20"/>
-      <c r="C22" s="32"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="32"/>
-      <c r="H22" s="32"/>
-      <c r="I22" s="33"/>
-      <c r="J22" s="34"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="34"/>
+      <c r="J22" s="35"/>
     </row>
     <row r="23" ht="15.75" customHeight="1"/>
     <row r="24" ht="15.75" customHeight="1"/>
@@ -2788,14 +2835,7 @@
     <row r="1012" ht="15.75" customHeight="1"/>
     <row r="1013" ht="15.75" customHeight="1"/>
   </sheetData>
-  <autoFilter ref="$A$1:$J$21">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="Friday Bible Study 7:00pm, Sunday Second Service 9:30am"/>
-        <filter val="Sunday Second Service 9:30am"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="$A$1:$J$21"/>
   <dataValidations>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:G21">
       <formula1>"UCI,CSULB,Biola,Chapman,Other"</formula1>
@@ -2851,212 +2891,214 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="36" t="s">
-        <v>101</v>
-      </c>
-      <c r="F1" s="36" t="s">
+      <c r="E1" s="37" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="G1" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="37" t="s">
+      <c r="I1" s="38" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="38">
+      <c r="A2" s="39">
         <v>45728.0</v>
       </c>
-      <c r="B2" s="39" t="s">
-        <v>102</v>
-      </c>
-      <c r="C2" s="39" t="s">
-        <v>103</v>
-      </c>
-      <c r="D2" s="39" t="s">
+      <c r="B2" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="E2" s="39">
+      <c r="C2" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="E2" s="40">
         <v>4.0</v>
       </c>
-      <c r="F2" s="39" t="s">
+      <c r="F2" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="40" t="s">
+      <c r="G2" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="39" t="s">
-        <v>105</v>
-      </c>
-      <c r="I2" s="41"/>
+      <c r="H2" s="40" t="s">
+        <v>107</v>
+      </c>
+      <c r="I2" s="42"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="38">
+      <c r="A3" s="39">
         <v>45729.0</v>
       </c>
-      <c r="B3" s="42" t="s">
-        <v>106</v>
-      </c>
-      <c r="C3" s="39" t="s">
-        <v>107</v>
-      </c>
-      <c r="D3" s="39" t="s">
+      <c r="B3" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="E3" s="39">
+      <c r="C3" s="40" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" s="40" t="s">
+        <v>110</v>
+      </c>
+      <c r="E3" s="40">
         <v>4.0</v>
       </c>
-      <c r="F3" s="39" t="s">
+      <c r="F3" s="40" t="s">
         <v>15</v>
       </c>
       <c r="G3" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="H3" s="42" t="s">
-        <v>109</v>
+      <c r="H3" s="40" t="s">
+        <v>111</v>
       </c>
       <c r="I3" s="44" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="38">
+      <c r="A4" s="39">
         <v>45730.0</v>
       </c>
-      <c r="B4" s="42" t="s">
-        <v>111</v>
-      </c>
-      <c r="C4" s="39" t="s">
-        <v>112</v>
-      </c>
-      <c r="D4" s="39" t="s">
+      <c r="B4" s="40" t="s">
         <v>113</v>
+      </c>
+      <c r="C4" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="D4" s="40" t="s">
+        <v>115</v>
       </c>
       <c r="E4" s="45">
         <v>2.0</v>
       </c>
-      <c r="F4" s="39" t="s">
+      <c r="F4" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="46" t="s">
+      <c r="G4" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="42" t="s">
-        <v>114</v>
-      </c>
-      <c r="I4" s="41"/>
+      <c r="H4" s="40" t="s">
+        <v>116</v>
+      </c>
+      <c r="I4" s="42"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="38">
+      <c r="A5" s="39">
         <v>45731.0</v>
       </c>
-      <c r="B5" s="42" t="s">
-        <v>115</v>
-      </c>
-      <c r="C5" s="39" t="s">
-        <v>116</v>
-      </c>
-      <c r="D5" s="39" t="s">
+      <c r="B5" s="40" t="s">
         <v>117</v>
       </c>
-      <c r="E5" s="39">
+      <c r="C5" s="40" t="s">
+        <v>118</v>
+      </c>
+      <c r="D5" s="40" t="s">
+        <v>119</v>
+      </c>
+      <c r="E5" s="40">
         <v>4.0</v>
       </c>
       <c r="F5" s="45" t="s">
         <v>51</v>
       </c>
       <c r="G5" s="43" t="s">
-        <v>44</v>
-      </c>
-      <c r="H5" s="47" t="s">
-        <v>118</v>
-      </c>
-      <c r="I5" s="41"/>
+        <v>21</v>
+      </c>
+      <c r="H5" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="I5" s="42"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="38">
+      <c r="A6" s="39">
         <v>45732.0</v>
       </c>
-      <c r="B6" s="47" t="s">
-        <v>119</v>
-      </c>
-      <c r="C6" s="39" t="s">
-        <v>120</v>
-      </c>
-      <c r="D6" s="39" t="s">
+      <c r="B6" s="45" t="s">
         <v>121</v>
+      </c>
+      <c r="C6" s="40" t="s">
+        <v>122</v>
+      </c>
+      <c r="D6" s="40" t="s">
+        <v>123</v>
       </c>
       <c r="E6" s="45">
         <v>6.0</v>
       </c>
-      <c r="F6" s="39" t="s">
+      <c r="F6" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="48" t="s">
+      <c r="G6" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="H6" s="47" t="s">
-        <v>122</v>
-      </c>
-      <c r="I6" s="41"/>
+      <c r="H6" s="45" t="s">
+        <v>124</v>
+      </c>
+      <c r="I6" s="44" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="38">
+      <c r="A7" s="39">
         <v>45733.0</v>
       </c>
-      <c r="B7" s="47" t="s">
-        <v>123</v>
-      </c>
-      <c r="C7" s="39" t="s">
-        <v>124</v>
-      </c>
-      <c r="D7" s="39" t="s">
-        <v>125</v>
+      <c r="B7" s="45" t="s">
+        <v>126</v>
+      </c>
+      <c r="C7" s="40" t="s">
+        <v>127</v>
+      </c>
+      <c r="D7" s="40" t="s">
+        <v>128</v>
       </c>
       <c r="E7" s="45">
         <v>3.0</v>
       </c>
       <c r="F7" s="45" t="s">
+        <v>77</v>
+      </c>
+      <c r="G7" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="G7" s="39" t="s">
-        <v>21</v>
-      </c>
-      <c r="H7" s="47" t="s">
-        <v>75</v>
-      </c>
-      <c r="I7" s="41"/>
+      <c r="I7" s="42"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="38">
+      <c r="A8" s="39">
         <v>45734.0</v>
       </c>
       <c r="B8" s="47" t="s">
-        <v>126</v>
-      </c>
-      <c r="C8" s="39" t="s">
-        <v>127</v>
-      </c>
-      <c r="D8" s="39" t="s">
-        <v>128</v>
-      </c>
-      <c r="E8" s="39">
+        <v>129</v>
+      </c>
+      <c r="C8" s="40" t="s">
+        <v>130</v>
+      </c>
+      <c r="D8" s="40" t="s">
+        <v>131</v>
+      </c>
+      <c r="E8" s="40">
         <v>4.0</v>
       </c>
       <c r="F8" s="47" t="s">
@@ -3066,45 +3108,63 @@
         <v>55</v>
       </c>
       <c r="H8" s="47" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="I8" s="44" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="49">
+      <c r="A9" s="48">
         <v>45735.0</v>
       </c>
-      <c r="B9" s="50" t="s">
-        <v>131</v>
-      </c>
-      <c r="C9" s="50" t="s">
-        <v>132</v>
-      </c>
-      <c r="D9" s="50" t="s">
-        <v>133</v>
-      </c>
-      <c r="E9" s="51">
+      <c r="B9" s="49" t="s">
+        <v>134</v>
+      </c>
+      <c r="C9" s="49" t="s">
+        <v>135</v>
+      </c>
+      <c r="D9" s="49" t="s">
+        <v>136</v>
+      </c>
+      <c r="E9" s="50">
         <v>4.0</v>
       </c>
-      <c r="F9" s="50" t="s">
-        <v>91</v>
-      </c>
-      <c r="G9" s="51" t="s">
+      <c r="F9" s="49" t="s">
+        <v>93</v>
+      </c>
+      <c r="G9" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="H9" s="50" t="s">
-        <v>134</v>
-      </c>
-      <c r="I9" s="52"/>
+      <c r="H9" s="49" t="s">
+        <v>137</v>
+      </c>
+      <c r="I9" s="51"/>
     </row>
     <row r="10" ht="15.75" customHeight="1"/>
-    <row r="11" ht="15.75" customHeight="1"/>
-    <row r="12" ht="15.75" customHeight="1"/>
-    <row r="13" ht="15.75" customHeight="1"/>
-    <row r="14" ht="15.75" customHeight="1"/>
-    <row r="15" ht="15.75" customHeight="1"/>
+    <row r="11" ht="15.75" customHeight="1">
+      <c r="B11" s="52"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="52"/>
+    </row>
+    <row r="12" ht="15.75" customHeight="1">
+      <c r="B12" s="52"/>
+      <c r="G12" s="54"/>
+      <c r="H12" s="52"/>
+    </row>
+    <row r="13" ht="15.75" customHeight="1">
+      <c r="B13" s="52"/>
+      <c r="G13" s="55"/>
+      <c r="H13" s="47"/>
+    </row>
+    <row r="14" ht="15.75" customHeight="1">
+      <c r="B14" s="47"/>
+      <c r="H14" s="47"/>
+    </row>
+    <row r="15" ht="15.75" customHeight="1">
+      <c r="B15" s="47"/>
+      <c r="H15" s="47"/>
+    </row>
     <row r="16" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
@@ -4099,8 +4159,10 @@
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait"/>
   <drawing r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId3"/>
+  <tableParts count="3">
+    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>